<commit_message>
Signed-off-by: yasumasakataoka Signed-off-by: yasumasakataoka Signed-off-by: yasumasakataoka
</commit_message>
<xml_diff>
--- a/vendor/OrorBlk/帳票サンプル2.xlsx
+++ b/vendor/OrorBlk/帳票サンプル2.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="20730" windowHeight="11175"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="R_ITMS" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>:itm_code</t>
     <phoneticPr fontId="1"/>
@@ -33,19 +33,36 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>fff</t>
+    <t>品目コード</t>
+    <rPh sb="0" eb="2">
+      <t>ヒンモク</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ggg</t>
+    <t>品名</t>
+    <rPh sb="0" eb="2">
+      <t>ヒンメイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>xxxxxxxxxxxxx</t>
+    <t>す</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>xxxxxxxxxxxxxxx</t>
+    <t>備考</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>:itm_code;1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>:itm_remark;0#</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -53,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,16 +118,54 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -191,10 +246,97 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0070C0"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -203,68 +345,207 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thick">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
+      <right style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FFC00000"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
+      </left>
       <right/>
       <top style="thin">
-        <color rgb="FFC00000"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
+      <right style="thin">
+        <color theme="3" tint="0.39994506668294322"/>
       </right>
       <top style="thin">
-        <color rgb="FFC00000"/>
+        <color rgb="FFFF0000"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -275,7 +556,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -300,82 +581,178 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -384,6 +761,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF3347D9"/>
+      <color rgb="FF000000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -679,11 +1063,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AY36"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:BB36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK6" sqref="AK6"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -696,26 +1081,24 @@
     <col min="62" max="63" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:54" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:54" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -737,7 +1120,7 @@
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
     </row>
-    <row r="3" spans="1:51" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:54" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -772,30 +1155,28 @@
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
-      <c r="AH3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="12"/>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="12"/>
-      <c r="AU3" s="13"/>
-    </row>
-    <row r="4" spans="1:51" ht="32.25" x14ac:dyDescent="0.15">
-      <c r="A4" s="26" t="s">
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24"/>
+      <c r="AL3" s="24"/>
+      <c r="AM3" s="24"/>
+      <c r="AN3" s="24"/>
+      <c r="AO3" s="24"/>
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="24"/>
+      <c r="AR3" s="24"/>
+      <c r="AS3" s="24"/>
+      <c r="AT3" s="24"/>
+      <c r="AU3" s="30"/>
+    </row>
+    <row r="4" spans="1:54" ht="32.25" x14ac:dyDescent="0.15">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -824,28 +1205,30 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
-      <c r="AO4" s="15"/>
-      <c r="AP4" s="15"/>
-      <c r="AQ4" s="15"/>
-      <c r="AR4" s="15"/>
-      <c r="AS4" s="15"/>
-      <c r="AT4" s="15"/>
-      <c r="AU4" s="16"/>
-    </row>
-    <row r="5" spans="1:51" ht="32.25" x14ac:dyDescent="0.15">
-      <c r="A5" s="26" t="s">
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="11"/>
+      <c r="AQ4" s="11"/>
+      <c r="AR4" s="11"/>
+      <c r="AS4" s="11"/>
+      <c r="AT4" s="11"/>
+      <c r="AU4" s="31"/>
+    </row>
+    <row r="5" spans="1:54" ht="32.25" x14ac:dyDescent="0.15">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -874,28 +1257,28 @@
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="16"/>
-    </row>
-    <row r="6" spans="1:51" ht="32.25" x14ac:dyDescent="0.15">
-      <c r="A6" s="26" t="s">
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="11"/>
+      <c r="AM5" s="11"/>
+      <c r="AN5" s="11"/>
+      <c r="AO5" s="11"/>
+      <c r="AP5" s="11"/>
+      <c r="AQ5" s="11"/>
+      <c r="AR5" s="11"/>
+      <c r="AS5" s="11"/>
+      <c r="AT5" s="11"/>
+      <c r="AU5" s="31"/>
+    </row>
+    <row r="6" spans="1:54" ht="32.25" x14ac:dyDescent="0.15">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -924,28 +1307,28 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="16"/>
-    </row>
-    <row r="7" spans="1:51" ht="32.25" x14ac:dyDescent="0.15">
-      <c r="A7" s="26" t="s">
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="11"/>
+      <c r="AR6" s="11"/>
+      <c r="AS6" s="11"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="31"/>
+    </row>
+    <row r="7" spans="1:54" ht="32.25" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -974,28 +1357,28 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
-      <c r="AH7" s="14"/>
-      <c r="AI7" s="15"/>
-      <c r="AJ7" s="15"/>
-      <c r="AK7" s="15"/>
-      <c r="AL7" s="15"/>
-      <c r="AM7" s="15"/>
-      <c r="AN7" s="15"/>
-      <c r="AO7" s="15"/>
-      <c r="AP7" s="15"/>
-      <c r="AQ7" s="15"/>
-      <c r="AR7" s="15"/>
-      <c r="AS7" s="15"/>
-      <c r="AT7" s="15"/>
-      <c r="AU7" s="16"/>
-    </row>
-    <row r="8" spans="1:51" ht="33" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="11"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="11"/>
+      <c r="AP7" s="11"/>
+      <c r="AQ7" s="11"/>
+      <c r="AR7" s="11"/>
+      <c r="AS7" s="11"/>
+      <c r="AT7" s="11"/>
+      <c r="AU7" s="31"/>
+    </row>
+    <row r="8" spans="1:54" ht="33" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1024,23 +1407,23 @@
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
-      <c r="AH8" s="17"/>
-      <c r="AI8" s="18"/>
-      <c r="AJ8" s="18"/>
-      <c r="AK8" s="18"/>
-      <c r="AL8" s="18"/>
-      <c r="AM8" s="18"/>
-      <c r="AN8" s="18"/>
-      <c r="AO8" s="18"/>
-      <c r="AP8" s="18"/>
-      <c r="AQ8" s="18"/>
-      <c r="AR8" s="18"/>
-      <c r="AS8" s="18"/>
-      <c r="AT8" s="18"/>
-      <c r="AU8" s="19"/>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.15">
-      <c r="A9" s="26" t="s">
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="11"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="11"/>
+      <c r="AP8" s="11"/>
+      <c r="AQ8" s="11"/>
+      <c r="AR8" s="11"/>
+      <c r="AS8" s="11"/>
+      <c r="AT8" s="11"/>
+      <c r="AU8" s="32"/>
+    </row>
+    <row r="9" spans="1:54" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="4"/>
@@ -1069,109 +1452,127 @@
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.15">
-      <c r="A10" s="26" t="s">
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="13"/>
+      <c r="AM9" s="13"/>
+      <c r="AN9" s="13"/>
+      <c r="AO9" s="13"/>
+      <c r="AP9" s="13"/>
+      <c r="AQ9" s="13"/>
+      <c r="AR9" s="13"/>
+      <c r="AS9" s="13"/>
+      <c r="AT9" s="13"/>
+      <c r="AU9" s="13"/>
+    </row>
+    <row r="10" spans="1:54" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.15">
-      <c r="A11" s="26">
+      <c r="AY10" s="4"/>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="A11" s="12">
         <v>1</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="20" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21"/>
-      <c r="AE11" s="21"/>
-      <c r="AF11" s="21"/>
-      <c r="AG11" s="21"/>
-      <c r="AH11" s="21"/>
-      <c r="AI11" s="22"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="2" t="s">
+      <c r="X11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="Z11" s="36"/>
+      <c r="AA11" s="36"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="27"/>
+      <c r="AJ11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="AL11" s="2"/>
-      <c r="AM11" s="2"/>
-      <c r="AN11" s="2"/>
-      <c r="AO11" s="2"/>
-      <c r="AP11" s="2"/>
-      <c r="AQ11" s="2"/>
-      <c r="AR11" s="2"/>
-      <c r="AS11" s="2"/>
-      <c r="AT11" s="2"/>
-      <c r="AU11" s="2"/>
-      <c r="AV11" s="2"/>
-      <c r="AW11" s="3"/>
-      <c r="AY11" s="8"/>
-    </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.15">
-      <c r="A12" s="26"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="24"/>
-      <c r="AE12" s="24"/>
-      <c r="AF12" s="24"/>
-      <c r="AG12" s="24"/>
-      <c r="AH12" s="24"/>
-      <c r="AI12" s="25"/>
-      <c r="AJ12" s="5"/>
+      <c r="AK11" s="18"/>
+      <c r="AL11" s="18"/>
+      <c r="AM11" s="18"/>
+      <c r="AN11" s="18"/>
+      <c r="AO11" s="18"/>
+      <c r="AP11" s="18"/>
+      <c r="AQ11" s="18"/>
+      <c r="AR11" s="18"/>
+      <c r="AS11" s="18"/>
+      <c r="AT11" s="18"/>
+      <c r="AU11" s="18"/>
+      <c r="AV11" s="18"/>
+      <c r="AW11" s="19"/>
+      <c r="AY11" s="4"/>
+      <c r="AZ11" s="4"/>
+      <c r="BA11" s="4"/>
+      <c r="BB11" s="4"/>
+    </row>
+    <row r="12" spans="1:54" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="29"/>
+      <c r="AJ12" s="6"/>
       <c r="AK12" s="6"/>
       <c r="AL12" s="6"/>
       <c r="AM12" s="6"/>
@@ -1185,118 +1586,129 @@
       <c r="AU12" s="6"/>
       <c r="AV12" s="6"/>
       <c r="AW12" s="7"/>
-    </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.15">
-      <c r="A13" s="26">
+      <c r="AY12" s="4"/>
+      <c r="AZ12" s="4"/>
+      <c r="BA12" s="4"/>
+      <c r="BB12" s="4"/>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="A13" s="12">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="27" t="s">
+      <c r="B13" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
-      <c r="AG13" s="28"/>
-      <c r="AH13" s="28"/>
-      <c r="AI13" s="29"/>
-      <c r="AJ13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="2"/>
-      <c r="AP13" s="2"/>
-      <c r="AQ13" s="2"/>
-      <c r="AR13" s="2"/>
-      <c r="AS13" s="2"/>
-      <c r="AT13" s="2"/>
-      <c r="AU13" s="2"/>
-      <c r="AV13" s="2"/>
-      <c r="AW13" s="3"/>
-      <c r="AY13" s="8"/>
-    </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.15">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
-      <c r="AC14" s="31"/>
-      <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="31"/>
-      <c r="AI14" s="32"/>
-      <c r="AJ14" s="5"/>
-      <c r="AK14" s="6"/>
-      <c r="AL14" s="6"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
-      <c r="AO14" s="6"/>
-      <c r="AP14" s="6"/>
-      <c r="AQ14" s="6"/>
-      <c r="AR14" s="6"/>
-      <c r="AS14" s="6"/>
-      <c r="AT14" s="6"/>
-      <c r="AU14" s="6"/>
-      <c r="AV14" s="6"/>
-      <c r="AW14" s="7"/>
-    </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="50"/>
+      <c r="AF13" s="50"/>
+      <c r="AG13" s="50"/>
+      <c r="AH13" s="50"/>
+      <c r="AI13" s="51"/>
+      <c r="AJ13" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK13" s="40"/>
+      <c r="AL13" s="40"/>
+      <c r="AM13" s="40"/>
+      <c r="AN13" s="40"/>
+      <c r="AO13" s="40"/>
+      <c r="AP13" s="40"/>
+      <c r="AQ13" s="40"/>
+      <c r="AR13" s="40"/>
+      <c r="AS13" s="40"/>
+      <c r="AT13" s="40"/>
+      <c r="AU13" s="40"/>
+      <c r="AV13" s="40"/>
+      <c r="AW13" s="41"/>
+      <c r="AY13" s="4"/>
+      <c r="AZ13" s="4"/>
+      <c r="BA13" s="4"/>
+      <c r="BB13" s="4"/>
+    </row>
+    <row r="14" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="B14" s="42"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="53"/>
+      <c r="Z14" s="53"/>
+      <c r="AA14" s="53"/>
+      <c r="AB14" s="53"/>
+      <c r="AC14" s="53"/>
+      <c r="AD14" s="53"/>
+      <c r="AE14" s="53"/>
+      <c r="AF14" s="53"/>
+      <c r="AG14" s="53"/>
+      <c r="AH14" s="53"/>
+      <c r="AI14" s="54"/>
+      <c r="AJ14" s="43"/>
+      <c r="AK14" s="43"/>
+      <c r="AL14" s="43"/>
+      <c r="AM14" s="43"/>
+      <c r="AN14" s="43"/>
+      <c r="AO14" s="43"/>
+      <c r="AP14" s="43"/>
+      <c r="AQ14" s="43"/>
+      <c r="AR14" s="43"/>
+      <c r="AS14" s="43"/>
+      <c r="AT14" s="43"/>
+      <c r="AU14" s="43"/>
+      <c r="AV14" s="43"/>
+      <c r="AW14" s="45"/>
+      <c r="AY14" s="4"/>
+      <c r="AZ14" s="4"/>
+      <c r="BA14" s="4"/>
+      <c r="BB14" s="4"/>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1308,9 +1720,9 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -1318,27 +1730,25 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
-      <c r="AA15" s="28"/>
-      <c r="AB15" s="28"/>
-      <c r="AC15" s="28"/>
-      <c r="AD15" s="28"/>
-      <c r="AE15" s="28"/>
-      <c r="AF15" s="28"/>
-      <c r="AG15" s="28"/>
-      <c r="AH15" s="28"/>
-      <c r="AI15" s="29"/>
-      <c r="AJ15" s="1" t="s">
+      <c r="R15" s="55"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="56"/>
+      <c r="X15" s="56"/>
+      <c r="Y15" s="56"/>
+      <c r="Z15" s="56"/>
+      <c r="AA15" s="56"/>
+      <c r="AB15" s="56"/>
+      <c r="AC15" s="56"/>
+      <c r="AD15" s="56"/>
+      <c r="AE15" s="56"/>
+      <c r="AF15" s="56"/>
+      <c r="AG15" s="56"/>
+      <c r="AH15" s="56"/>
+      <c r="AI15" s="57"/>
+      <c r="AJ15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK15" s="2"/>
@@ -1354,18 +1764,21 @@
       <c r="AU15" s="2"/>
       <c r="AV15" s="2"/>
       <c r="AW15" s="3"/>
-      <c r="AY15" s="8"/>
-    </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY15" s="4"/>
+      <c r="AZ15" s="4"/>
+      <c r="BA15" s="4"/>
+      <c r="BB15" s="4"/>
+    </row>
+    <row r="16" spans="1:54" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
@@ -1373,25 +1786,25 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="31"/>
-      <c r="Z16" s="31"/>
-      <c r="AA16" s="31"/>
-      <c r="AB16" s="31"/>
-      <c r="AC16" s="31"/>
-      <c r="AD16" s="31"/>
-      <c r="AE16" s="31"/>
-      <c r="AF16" s="31"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="31"/>
-      <c r="AI16" s="32"/>
-      <c r="AJ16" s="5"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="59"/>
+      <c r="U16" s="59"/>
+      <c r="V16" s="59"/>
+      <c r="W16" s="59"/>
+      <c r="X16" s="59"/>
+      <c r="Y16" s="59"/>
+      <c r="Z16" s="59"/>
+      <c r="AA16" s="59"/>
+      <c r="AB16" s="59"/>
+      <c r="AC16" s="59"/>
+      <c r="AD16" s="59"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="59"/>
+      <c r="AG16" s="59"/>
+      <c r="AH16" s="59"/>
+      <c r="AI16" s="60"/>
+      <c r="AJ16" s="6"/>
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
       <c r="AM16" s="6"/>
@@ -1405,8 +1818,12 @@
       <c r="AU16" s="6"/>
       <c r="AV16" s="6"/>
       <c r="AW16" s="7"/>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY16" s="4"/>
+      <c r="AZ16" s="4"/>
+      <c r="BA16" s="4"/>
+      <c r="BB16" s="4"/>
+    </row>
+    <row r="17" spans="1:54" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1418,9 +1835,9 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -1428,27 +1845,27 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-      <c r="R17" s="27" t="s">
+      <c r="R17" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="28"/>
-      <c r="Z17" s="28"/>
-      <c r="AA17" s="28"/>
-      <c r="AB17" s="28"/>
-      <c r="AC17" s="28"/>
-      <c r="AD17" s="28"/>
-      <c r="AE17" s="28"/>
-      <c r="AF17" s="28"/>
-      <c r="AG17" s="28"/>
-      <c r="AH17" s="28"/>
-      <c r="AI17" s="29"/>
-      <c r="AJ17" s="1" t="s">
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="48"/>
+      <c r="AC17" s="48"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="48"/>
+      <c r="AF17" s="48"/>
+      <c r="AG17" s="48"/>
+      <c r="AH17" s="48"/>
+      <c r="AI17" s="65"/>
+      <c r="AJ17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK17" s="2"/>
@@ -1464,18 +1881,21 @@
       <c r="AU17" s="2"/>
       <c r="AV17" s="2"/>
       <c r="AW17" s="3"/>
-      <c r="AY17" s="8"/>
-    </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY17" s="4"/>
+      <c r="AZ17" s="4"/>
+      <c r="BA17" s="4"/>
+      <c r="BB17" s="4"/>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
@@ -1483,25 +1903,25 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="31"/>
-      <c r="AC18" s="31"/>
-      <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-      <c r="AI18" s="32"/>
-      <c r="AJ18" s="5"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="62"/>
+      <c r="W18" s="62"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="62"/>
+      <c r="AA18" s="62"/>
+      <c r="AB18" s="62"/>
+      <c r="AC18" s="62"/>
+      <c r="AD18" s="62"/>
+      <c r="AE18" s="62"/>
+      <c r="AF18" s="62"/>
+      <c r="AG18" s="62"/>
+      <c r="AH18" s="62"/>
+      <c r="AI18" s="63"/>
+      <c r="AJ18" s="6"/>
       <c r="AK18" s="6"/>
       <c r="AL18" s="6"/>
       <c r="AM18" s="6"/>
@@ -1515,22 +1935,26 @@
       <c r="AU18" s="6"/>
       <c r="AV18" s="6"/>
       <c r="AW18" s="7"/>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY18" s="4"/>
+      <c r="AZ18" s="4"/>
+      <c r="BA18" s="4"/>
+      <c r="BB18" s="4"/>
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>4</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -1538,27 +1962,27 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="27" t="s">
+      <c r="R19" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
-      <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="Y19" s="28"/>
-      <c r="Z19" s="28"/>
-      <c r="AA19" s="28"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="28"/>
-      <c r="AD19" s="28"/>
-      <c r="AE19" s="28"/>
-      <c r="AF19" s="28"/>
-      <c r="AG19" s="28"/>
-      <c r="AH19" s="28"/>
-      <c r="AI19" s="29"/>
-      <c r="AJ19" s="1" t="s">
+      <c r="S19" s="56"/>
+      <c r="T19" s="56"/>
+      <c r="U19" s="56"/>
+      <c r="V19" s="56"/>
+      <c r="W19" s="56"/>
+      <c r="X19" s="56"/>
+      <c r="Y19" s="56"/>
+      <c r="Z19" s="56"/>
+      <c r="AA19" s="56"/>
+      <c r="AB19" s="56"/>
+      <c r="AC19" s="56"/>
+      <c r="AD19" s="56"/>
+      <c r="AE19" s="56"/>
+      <c r="AF19" s="56"/>
+      <c r="AG19" s="56"/>
+      <c r="AH19" s="56"/>
+      <c r="AI19" s="57"/>
+      <c r="AJ19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK19" s="2"/>
@@ -1574,18 +1998,21 @@
       <c r="AU19" s="2"/>
       <c r="AV19" s="2"/>
       <c r="AW19" s="3"/>
-      <c r="AY19" s="8"/>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY19" s="4"/>
+      <c r="AZ19" s="4"/>
+      <c r="BA19" s="4"/>
+      <c r="BB19" s="4"/>
+    </row>
+    <row r="20" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
@@ -1593,25 +2020,25 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
-      <c r="R20" s="30"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="31"/>
-      <c r="Z20" s="31"/>
-      <c r="AA20" s="31"/>
-      <c r="AB20" s="31"/>
-      <c r="AC20" s="31"/>
-      <c r="AD20" s="31"/>
-      <c r="AE20" s="31"/>
-      <c r="AF20" s="31"/>
-      <c r="AG20" s="31"/>
-      <c r="AH20" s="31"/>
-      <c r="AI20" s="32"/>
-      <c r="AJ20" s="5"/>
+      <c r="R20" s="61"/>
+      <c r="S20" s="62"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="62"/>
+      <c r="V20" s="62"/>
+      <c r="W20" s="62"/>
+      <c r="X20" s="62"/>
+      <c r="Y20" s="62"/>
+      <c r="Z20" s="62"/>
+      <c r="AA20" s="62"/>
+      <c r="AB20" s="62"/>
+      <c r="AC20" s="62"/>
+      <c r="AD20" s="62"/>
+      <c r="AE20" s="62"/>
+      <c r="AF20" s="62"/>
+      <c r="AG20" s="62"/>
+      <c r="AH20" s="62"/>
+      <c r="AI20" s="63"/>
+      <c r="AJ20" s="6"/>
       <c r="AK20" s="6"/>
       <c r="AL20" s="6"/>
       <c r="AM20" s="6"/>
@@ -1625,8 +2052,12 @@
       <c r="AU20" s="6"/>
       <c r="AV20" s="6"/>
       <c r="AW20" s="7"/>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY20" s="4"/>
+      <c r="AZ20" s="4"/>
+      <c r="BA20" s="4"/>
+      <c r="BB20" s="4"/>
+    </row>
+    <row r="21" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>5</v>
       </c>
@@ -1638,9 +2069,9 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
@@ -1648,27 +2079,27 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="27" t="s">
+      <c r="R21" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S21" s="28"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="28"/>
-      <c r="V21" s="28"/>
-      <c r="W21" s="28"/>
-      <c r="X21" s="28"/>
-      <c r="Y21" s="28"/>
-      <c r="Z21" s="28"/>
-      <c r="AA21" s="28"/>
-      <c r="AB21" s="28"/>
-      <c r="AC21" s="28"/>
-      <c r="AD21" s="28"/>
-      <c r="AE21" s="28"/>
-      <c r="AF21" s="28"/>
-      <c r="AG21" s="28"/>
-      <c r="AH21" s="28"/>
-      <c r="AI21" s="29"/>
-      <c r="AJ21" s="1" t="s">
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+      <c r="V21" s="56"/>
+      <c r="W21" s="56"/>
+      <c r="X21" s="56"/>
+      <c r="Y21" s="56"/>
+      <c r="Z21" s="56"/>
+      <c r="AA21" s="56"/>
+      <c r="AB21" s="56"/>
+      <c r="AC21" s="56"/>
+      <c r="AD21" s="56"/>
+      <c r="AE21" s="56"/>
+      <c r="AF21" s="56"/>
+      <c r="AG21" s="56"/>
+      <c r="AH21" s="56"/>
+      <c r="AI21" s="57"/>
+      <c r="AJ21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK21" s="2"/>
@@ -1684,18 +2115,21 @@
       <c r="AU21" s="2"/>
       <c r="AV21" s="2"/>
       <c r="AW21" s="3"/>
-      <c r="AY21" s="8"/>
-    </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY21" s="4"/>
+      <c r="AZ21" s="4"/>
+      <c r="BA21" s="4"/>
+      <c r="BB21" s="4"/>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
@@ -1703,25 +2137,25 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="31"/>
-      <c r="Z22" s="31"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="31"/>
-      <c r="AC22" s="31"/>
-      <c r="AD22" s="31"/>
-      <c r="AE22" s="31"/>
-      <c r="AF22" s="31"/>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="31"/>
-      <c r="AI22" s="32"/>
-      <c r="AJ22" s="5"/>
+      <c r="R22" s="61"/>
+      <c r="S22" s="62"/>
+      <c r="T22" s="62"/>
+      <c r="U22" s="62"/>
+      <c r="V22" s="62"/>
+      <c r="W22" s="62"/>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="62"/>
+      <c r="Z22" s="62"/>
+      <c r="AA22" s="62"/>
+      <c r="AB22" s="62"/>
+      <c r="AC22" s="62"/>
+      <c r="AD22" s="62"/>
+      <c r="AE22" s="62"/>
+      <c r="AF22" s="62"/>
+      <c r="AG22" s="62"/>
+      <c r="AH22" s="62"/>
+      <c r="AI22" s="63"/>
+      <c r="AJ22" s="6"/>
       <c r="AK22" s="6"/>
       <c r="AL22" s="6"/>
       <c r="AM22" s="6"/>
@@ -1735,8 +2169,12 @@
       <c r="AU22" s="6"/>
       <c r="AV22" s="6"/>
       <c r="AW22" s="7"/>
-    </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY22" s="4"/>
+      <c r="AZ22" s="4"/>
+      <c r="BA22" s="4"/>
+      <c r="BB22" s="4"/>
+    </row>
+    <row r="23" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>6</v>
       </c>
@@ -1748,9 +2186,9 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -1758,27 +2196,27 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-      <c r="R23" s="27" t="s">
+      <c r="R23" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="28"/>
-      <c r="AA23" s="28"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
-      <c r="AG23" s="28"/>
-      <c r="AH23" s="28"/>
-      <c r="AI23" s="29"/>
-      <c r="AJ23" s="1" t="s">
+      <c r="S23" s="56"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="56"/>
+      <c r="Y23" s="56"/>
+      <c r="Z23" s="56"/>
+      <c r="AA23" s="56"/>
+      <c r="AB23" s="56"/>
+      <c r="AC23" s="56"/>
+      <c r="AD23" s="56"/>
+      <c r="AE23" s="56"/>
+      <c r="AF23" s="56"/>
+      <c r="AG23" s="56"/>
+      <c r="AH23" s="56"/>
+      <c r="AI23" s="57"/>
+      <c r="AJ23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK23" s="2"/>
@@ -1794,18 +2232,21 @@
       <c r="AU23" s="2"/>
       <c r="AV23" s="2"/>
       <c r="AW23" s="3"/>
-      <c r="AY23" s="8"/>
-    </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY23" s="4"/>
+      <c r="AZ23" s="4"/>
+      <c r="BA23" s="4"/>
+      <c r="BB23" s="4"/>
+    </row>
+    <row r="24" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1813,25 +2254,25 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="31"/>
-      <c r="Z24" s="31"/>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="31"/>
-      <c r="AC24" s="31"/>
-      <c r="AD24" s="31"/>
-      <c r="AE24" s="31"/>
-      <c r="AF24" s="31"/>
-      <c r="AG24" s="31"/>
-      <c r="AH24" s="31"/>
-      <c r="AI24" s="32"/>
-      <c r="AJ24" s="5"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="62"/>
+      <c r="T24" s="62"/>
+      <c r="U24" s="62"/>
+      <c r="V24" s="62"/>
+      <c r="W24" s="62"/>
+      <c r="X24" s="62"/>
+      <c r="Y24" s="62"/>
+      <c r="Z24" s="62"/>
+      <c r="AA24" s="62"/>
+      <c r="AB24" s="62"/>
+      <c r="AC24" s="62"/>
+      <c r="AD24" s="62"/>
+      <c r="AE24" s="62"/>
+      <c r="AF24" s="62"/>
+      <c r="AG24" s="62"/>
+      <c r="AH24" s="62"/>
+      <c r="AI24" s="63"/>
+      <c r="AJ24" s="6"/>
       <c r="AK24" s="6"/>
       <c r="AL24" s="6"/>
       <c r="AM24" s="6"/>
@@ -1845,8 +2286,12 @@
       <c r="AU24" s="6"/>
       <c r="AV24" s="6"/>
       <c r="AW24" s="7"/>
-    </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY24" s="4"/>
+      <c r="AZ24" s="4"/>
+      <c r="BA24" s="4"/>
+      <c r="BB24" s="4"/>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>7</v>
       </c>
@@ -1858,9 +2303,9 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1868,27 +2313,27 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="27" t="s">
+      <c r="R25" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="28"/>
-      <c r="AH25" s="28"/>
-      <c r="AI25" s="29"/>
-      <c r="AJ25" s="1" t="s">
+      <c r="S25" s="56"/>
+      <c r="T25" s="56"/>
+      <c r="U25" s="56"/>
+      <c r="V25" s="56"/>
+      <c r="W25" s="56"/>
+      <c r="X25" s="56"/>
+      <c r="Y25" s="56"/>
+      <c r="Z25" s="56"/>
+      <c r="AA25" s="56"/>
+      <c r="AB25" s="56"/>
+      <c r="AC25" s="56"/>
+      <c r="AD25" s="56"/>
+      <c r="AE25" s="56"/>
+      <c r="AF25" s="56"/>
+      <c r="AG25" s="56"/>
+      <c r="AH25" s="56"/>
+      <c r="AI25" s="57"/>
+      <c r="AJ25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK25" s="2"/>
@@ -1904,18 +2349,21 @@
       <c r="AU25" s="2"/>
       <c r="AV25" s="2"/>
       <c r="AW25" s="3"/>
-      <c r="AY25" s="8"/>
-    </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY25" s="4"/>
+      <c r="AZ25" s="4"/>
+      <c r="BA25" s="4"/>
+      <c r="BB25" s="4"/>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
@@ -1923,25 +2371,25 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="31"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31"/>
-      <c r="AG26" s="31"/>
-      <c r="AH26" s="31"/>
-      <c r="AI26" s="32"/>
-      <c r="AJ26" s="5"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="62"/>
+      <c r="T26" s="62"/>
+      <c r="U26" s="62"/>
+      <c r="V26" s="62"/>
+      <c r="W26" s="62"/>
+      <c r="X26" s="62"/>
+      <c r="Y26" s="62"/>
+      <c r="Z26" s="62"/>
+      <c r="AA26" s="62"/>
+      <c r="AB26" s="62"/>
+      <c r="AC26" s="62"/>
+      <c r="AD26" s="62"/>
+      <c r="AE26" s="62"/>
+      <c r="AF26" s="62"/>
+      <c r="AG26" s="62"/>
+      <c r="AH26" s="62"/>
+      <c r="AI26" s="63"/>
+      <c r="AJ26" s="6"/>
       <c r="AK26" s="6"/>
       <c r="AL26" s="6"/>
       <c r="AM26" s="6"/>
@@ -1955,8 +2403,12 @@
       <c r="AU26" s="6"/>
       <c r="AV26" s="6"/>
       <c r="AW26" s="7"/>
-    </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY26" s="4"/>
+      <c r="AZ26" s="4"/>
+      <c r="BA26" s="4"/>
+      <c r="BB26" s="4"/>
+    </row>
+    <row r="27" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1968,9 +2420,9 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
@@ -1978,27 +2430,27 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
-      <c r="R27" s="27" t="s">
+      <c r="R27" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S27" s="28"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="28"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="28"/>
-      <c r="Z27" s="28"/>
-      <c r="AA27" s="28"/>
-      <c r="AB27" s="28"/>
-      <c r="AC27" s="28"/>
-      <c r="AD27" s="28"/>
-      <c r="AE27" s="28"/>
-      <c r="AF27" s="28"/>
-      <c r="AG27" s="28"/>
-      <c r="AH27" s="28"/>
-      <c r="AI27" s="29"/>
-      <c r="AJ27" s="1" t="s">
+      <c r="S27" s="56"/>
+      <c r="T27" s="56"/>
+      <c r="U27" s="56"/>
+      <c r="V27" s="56"/>
+      <c r="W27" s="56"/>
+      <c r="X27" s="56"/>
+      <c r="Y27" s="56"/>
+      <c r="Z27" s="56"/>
+      <c r="AA27" s="56"/>
+      <c r="AB27" s="56"/>
+      <c r="AC27" s="56"/>
+      <c r="AD27" s="56"/>
+      <c r="AE27" s="56"/>
+      <c r="AF27" s="56"/>
+      <c r="AG27" s="56"/>
+      <c r="AH27" s="56"/>
+      <c r="AI27" s="57"/>
+      <c r="AJ27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="AK27" s="2"/>
@@ -2014,18 +2466,21 @@
       <c r="AU27" s="2"/>
       <c r="AV27" s="2"/>
       <c r="AW27" s="3"/>
-      <c r="AY27" s="8"/>
-    </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY27" s="4"/>
+      <c r="AZ27" s="4"/>
+      <c r="BA27" s="4"/>
+      <c r="BB27" s="4"/>
+    </row>
+    <row r="28" spans="1:54" x14ac:dyDescent="0.15">
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
@@ -2033,25 +2488,25 @@
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
-      <c r="X28" s="31"/>
-      <c r="Y28" s="31"/>
-      <c r="Z28" s="31"/>
-      <c r="AA28" s="31"/>
-      <c r="AB28" s="31"/>
-      <c r="AC28" s="31"/>
-      <c r="AD28" s="31"/>
-      <c r="AE28" s="31"/>
-      <c r="AF28" s="31"/>
-      <c r="AG28" s="31"/>
-      <c r="AH28" s="31"/>
-      <c r="AI28" s="32"/>
-      <c r="AJ28" s="5"/>
+      <c r="R28" s="61"/>
+      <c r="S28" s="62"/>
+      <c r="T28" s="62"/>
+      <c r="U28" s="62"/>
+      <c r="V28" s="62"/>
+      <c r="W28" s="62"/>
+      <c r="X28" s="62"/>
+      <c r="Y28" s="62"/>
+      <c r="Z28" s="62"/>
+      <c r="AA28" s="62"/>
+      <c r="AB28" s="62"/>
+      <c r="AC28" s="62"/>
+      <c r="AD28" s="62"/>
+      <c r="AE28" s="62"/>
+      <c r="AF28" s="62"/>
+      <c r="AG28" s="62"/>
+      <c r="AH28" s="62"/>
+      <c r="AI28" s="63"/>
+      <c r="AJ28" s="6"/>
       <c r="AK28" s="6"/>
       <c r="AL28" s="6"/>
       <c r="AM28" s="6"/>
@@ -2065,8 +2520,12 @@
       <c r="AU28" s="6"/>
       <c r="AV28" s="6"/>
       <c r="AW28" s="7"/>
-    </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY28" s="4"/>
+      <c r="AZ28" s="4"/>
+      <c r="BA28" s="4"/>
+      <c r="BB28" s="4"/>
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2116,8 +2575,12 @@
       <c r="AU29" s="4"/>
       <c r="AV29" s="4"/>
       <c r="AW29" s="4"/>
-    </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY29" s="4"/>
+      <c r="AZ29" s="4"/>
+      <c r="BA29" s="4"/>
+      <c r="BB29" s="4"/>
+    </row>
+    <row r="30" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2167,8 +2630,12 @@
       <c r="AU30" s="4"/>
       <c r="AV30" s="4"/>
       <c r="AW30" s="4"/>
-    </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY30" s="4"/>
+      <c r="AZ30" s="4"/>
+      <c r="BA30" s="4"/>
+      <c r="BB30" s="4"/>
+    </row>
+    <row r="31" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2218,8 +2685,12 @@
       <c r="AU31" s="4"/>
       <c r="AV31" s="4"/>
       <c r="AW31" s="4"/>
-    </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.15">
+      <c r="AY31" s="4"/>
+      <c r="AZ31" s="4"/>
+      <c r="BA31" s="4"/>
+      <c r="BB31" s="4"/>
+    </row>
+    <row r="32" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2269,6 +2740,10 @@
       <c r="AU32" s="4"/>
       <c r="AV32" s="4"/>
       <c r="AW32" s="4"/>
+      <c r="AY32" s="4"/>
+      <c r="AZ32" s="4"/>
+      <c r="BA32" s="4"/>
+      <c r="BB32" s="4"/>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
@@ -2488,6 +2963,6 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>